<commit_message>
Pre-final version of v1.1 specs
Thoroughly reworked specs - last clarifications added 04/09/2015.

Database refactoring and field mapping tables remain to be discussed,
will be tackled next.
</commit_message>
<xml_diff>
--- a/database-info/Fada-use-of-tables-and-view.xlsx
+++ b/database-info/Fada-use-of-tables-and-view.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26207"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaikedewever/Documents/fada-import-specs/database-info/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="32620" windowHeight="22860"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32620" windowHeight="22860"/>
   </bookViews>
   <sheets>
     <sheet name="TABLES" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="0">"TABLES"</definedName>
   </definedNames>
-  <calcPr calcId="140001" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <webPublishing css="0" allowPng="1" codePage="1252"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="83">
   <si>
     <t>NameOfObject</t>
   </si>
@@ -270,6 +275,9 @@
   </si>
   <si>
     <t>Surprised to see these here as these are "import tables" - Reason?</t>
+  </si>
+  <si>
+    <t>Surprised to see this is in use, as I understood it was only created when the Rotifera data were processed &gt; possibility to reconcile together with greferences table??</t>
   </si>
 </sst>
 </file>
@@ -343,6 +351,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -674,24 +687,24 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.796875" customWidth="1"/>
+    <col min="2" max="2" width="25.796875" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" customWidth="1"/>
+    <col min="4" max="4" width="22.796875" customWidth="1"/>
+    <col min="5" max="5" width="10.796875" customWidth="1"/>
+    <col min="6" max="6" width="22.796875" customWidth="1"/>
+    <col min="7" max="7" width="10.796875" customWidth="1"/>
+    <col min="8" max="8" width="22.796875" customWidth="1"/>
+    <col min="9" max="9" width="10.796875" customWidth="1"/>
+    <col min="10" max="10" width="22.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -723,7 +736,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -744,7 +757,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -765,7 +778,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -786,7 +799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -803,7 +816,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -824,7 +837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -845,7 +858,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -864,7 +877,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -881,7 +894,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -898,7 +911,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -919,7 +932,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -940,7 +953,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
@@ -960,7 +973,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -983,7 +996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -1002,7 +1015,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1019,7 +1032,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -1038,7 +1051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
@@ -1057,7 +1070,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
@@ -1074,7 +1087,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
@@ -1095,7 +1108,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
@@ -1116,7 +1129,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>1</v>
       </c>
@@ -1133,7 +1146,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
@@ -1143,7 +1156,9 @@
       <c r="C23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="E23" s="1" t="s">
         <v>2</v>
       </c>
@@ -1157,7 +1172,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
@@ -1178,7 +1193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
@@ -1201,7 +1216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
@@ -1224,7 +1239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -1241,7 +1256,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>1</v>
       </c>
@@ -1258,7 +1273,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
@@ -1275,7 +1290,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
@@ -1298,7 +1313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
@@ -1317,7 +1332,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
@@ -1338,7 +1353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
@@ -1363,7 +1378,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
@@ -1384,7 +1399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
@@ -1401,7 +1416,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>3</v>
       </c>
@@ -1416,7 +1431,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
@@ -1431,7 +1446,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>3</v>
       </c>
@@ -1451,7 +1466,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
@@ -1471,7 +1486,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
@@ -1488,7 +1503,7 @@
       </c>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>3</v>
       </c>
@@ -1503,7 +1518,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>3</v>
       </c>
@@ -1520,7 +1535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>3</v>
       </c>
@@ -1537,7 +1552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>3</v>
       </c>
@@ -1552,7 +1567,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>3</v>
       </c>
@@ -1567,7 +1582,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>3</v>
       </c>
@@ -1582,7 +1597,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>3</v>
       </c>
@@ -1597,7 +1612,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>3</v>
       </c>
@@ -1612,7 +1627,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
@@ -1627,7 +1642,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>3</v>
       </c>
@@ -1647,7 +1662,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>3</v>
       </c>
@@ -1664,7 +1679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>3</v>
       </c>
@@ -1679,7 +1694,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
         <v>3</v>
       </c>
@@ -1694,7 +1709,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>3</v>
       </c>
@@ -1709,7 +1724,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>3</v>
       </c>
@@ -1728,10 +1743,5 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <pageMargins left="1" right="1" top="1.667" bottom="1.667" header="1" footer="1"/>
   <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
another small update to xls file
just syncing to be able to pick up the changes from home…
</commit_message>
<xml_diff>
--- a/database-info/Fada-use-of-tables-and-view.xlsx
+++ b/database-info/Fada-use-of-tables-and-view.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
-  <workbookPr date1904="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaikedewever/Documents/fada-import-specs/database-info/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17620"/>
   </bookViews>
   <sheets>
     <sheet name="TABLES" sheetId="1" r:id="rId1"/>
@@ -13,13 +18,50 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="0">"TABLES"</definedName>
   </definedNames>
-  <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
-  <webPublishing allowPng="1" css="0" codePage="1252"/>
+  <calcPr calcId="0" iterate="1" concurrentCalc="0"/>
+  <webPublishing css="0" allowPng="1" codePage="1252"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="C11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Only consulted</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7" count="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="79">
   <si>
     <t>FadaImport</t>
   </si>
@@ -40,36 +82,254 @@
   </si>
   <si>
     <t>Earlier version of DwC-A-export</t>
+  </si>
+  <si>
+    <t>TypeOfObject</t>
+  </si>
+  <si>
+    <t>NameOfObject</t>
+  </si>
+  <si>
+    <t>Remarks-FadaImport</t>
+  </si>
+  <si>
+    <t>FADA</t>
+  </si>
+  <si>
+    <t>Remarks-FADA</t>
+  </si>
+  <si>
+    <t>BioFresh</t>
+  </si>
+  <si>
+    <t>Remarks-BioFresh</t>
+  </si>
+  <si>
+    <t>DwC-A-export</t>
+  </si>
+  <si>
+    <t>Remarks-DwC-A-export</t>
+  </si>
+  <si>
+    <t>col.families</t>
+  </si>
+  <si>
+    <t>Surprised to see that this is directly used in the web-app</t>
+  </si>
+  <si>
+    <t>fada.archived_observations</t>
+  </si>
+  <si>
+    <t>fada.authors</t>
+  </si>
+  <si>
+    <t>fada.bassins</t>
+  </si>
+  <si>
+    <t>fada.biofresh_key_species</t>
+  </si>
+  <si>
+    <t>fada.biofresh_key_synonyms</t>
+  </si>
+  <si>
+    <t>fada.biofresh_key_taxons</t>
+  </si>
+  <si>
+    <t>fada.chapters</t>
+  </si>
+  <si>
+    <t>fada.conservations</t>
+  </si>
+  <si>
+    <t>fada.distributions</t>
+  </si>
+  <si>
+    <t>fada.greferences</t>
+  </si>
+  <si>
+    <t>fada.genus_to_family</t>
+  </si>
+  <si>
+    <t>Used in fada.fst_... Views</t>
+  </si>
+  <si>
+    <t>fada.groups</t>
+  </si>
+  <si>
+    <t>fada.groups_publications</t>
+  </si>
+  <si>
+    <t>fada.groups_taxons</t>
+  </si>
+  <si>
+    <t>fada.groups_users</t>
+  </si>
+  <si>
+    <t>fada.journals</t>
+  </si>
+  <si>
+    <t>Where used?</t>
+  </si>
+  <si>
+    <t>fada.locations</t>
+  </si>
+  <si>
+    <t>fada.observations</t>
+  </si>
+  <si>
+    <t>fada.observations_species</t>
+  </si>
+  <si>
+    <t>fada.obs_statuses</t>
+  </si>
+  <si>
+    <t>fada.publications</t>
+  </si>
+  <si>
+    <t>Surprised to see this is in use, as I understood it was only created when the Rotifera data were processed &gt; possibility to reconcile together with greferences table??</t>
+  </si>
+  <si>
+    <t>Not currently the case (Rotifera references stored in separate schema), but use is intended</t>
+  </si>
+  <si>
+    <t>fada.ranks</t>
+  </si>
+  <si>
+    <t>fada.regions</t>
+  </si>
+  <si>
+    <t>fada.regions_species</t>
+  </si>
+  <si>
+    <t>fada.roles</t>
+  </si>
+  <si>
+    <t>fada.roles_users</t>
+  </si>
+  <si>
+    <t>fada.sites</t>
+  </si>
+  <si>
+    <t>fada.species</t>
+  </si>
+  <si>
+    <t>fada.statuses</t>
+  </si>
+  <si>
+    <t>Wondering where this is used?</t>
+  </si>
+  <si>
+    <t>fada.synonyms</t>
+  </si>
+  <si>
+    <t>fada.taxons</t>
+  </si>
+  <si>
+    <t>fada.users</t>
+  </si>
+  <si>
+    <t>fada.versions</t>
+  </si>
+  <si>
+    <t>fada.biofresh_key_species_names</t>
+  </si>
+  <si>
+    <t>fada.fada_biofresh_export_id</t>
+  </si>
+  <si>
+    <t>fada.fada_export</t>
+  </si>
+  <si>
+    <t>fada.fada_export_region</t>
+  </si>
+  <si>
+    <t>fada.fadainfo</t>
+  </si>
+  <si>
+    <t>Surprised to see that none of these views is no longer in use, all directly called from BioFresh-portal app?</t>
+  </si>
+  <si>
+    <t>fada.families_with_no_htaxa</t>
+  </si>
+  <si>
+    <t>fada.fst_for_genus</t>
+  </si>
+  <si>
+    <t>fada.fst_for_tribe</t>
+  </si>
+  <si>
+    <t>fada.minitaxaview</t>
+  </si>
+  <si>
+    <t>fada.originalnames</t>
+  </si>
+  <si>
+    <t>fada.pubantoinsert</t>
+  </si>
+  <si>
+    <t>fada.pubsyntoinsert</t>
+  </si>
+  <si>
+    <t>fada.refscnames</t>
+  </si>
+  <si>
+    <t>fada.smallspecies</t>
+  </si>
+  <si>
+    <t>fada.species_crosstab</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Check, used for fst_for_genus OR genus_to_families table??</t>
+  </si>
+  <si>
+    <t>fada.synonyms_split</t>
+  </si>
+  <si>
+    <t>fada.view_groups</t>
+  </si>
+  <si>
+    <t>fada.view_regions</t>
+  </si>
+  <si>
+    <t>fada.view_species</t>
+  </si>
+  <si>
+    <t>fada.view_taxons</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
-      <sz val="10"/>
-      <strike val="0"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
+      <sz val="10"/>
       <color rgb="FFFF6600"/>
       <name val="Sans"/>
-      <sz val="10"/>
-      <strike val="0"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Sans"/>
+    </font>
+    <font>
       <sz val="10"/>
-      <strike val="0"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,128 +341,384 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="0" diagonalDown="0">
-      <left style="none">
-        <color rgb="FFC7C7C7"/>
-      </left>
-      <right style="none">
-        <color rgb="FFC7C7C7"/>
-      </right>
-      <top style="none">
-        <color rgb="FFC7C7C7"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FFC7C7C7"/>
-      </bottom>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.79688" customWidth="1"/>
-    <col min="2" max="2" width="25.79688" customWidth="1"/>
-    <col min="3" max="3" width="10.79688" customWidth="1"/>
-    <col min="4" max="4" width="22.79688" customWidth="1"/>
-    <col min="5" max="5" width="10.79688" customWidth="1"/>
-    <col min="6" max="6" width="22.79688" customWidth="1"/>
-    <col min="7" max="7" width="10.79688" customWidth="1"/>
-    <col min="8" max="8" width="22.79688" customWidth="1"/>
-    <col min="9" max="9" width="10.79688" customWidth="1"/>
-    <col min="10" max="10" width="22.79688" customWidth="1"/>
+    <col min="1" max="1" width="10.796875" customWidth="1"/>
+    <col min="2" max="2" width="25.796875" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" customWidth="1"/>
+    <col min="4" max="4" width="22.796875" customWidth="1"/>
+    <col min="5" max="5" width="10.796875" customWidth="1"/>
+    <col min="6" max="6" width="22.796875" customWidth="1"/>
+    <col min="7" max="7" width="10.796875" customWidth="1"/>
+    <col min="8" max="8" width="22.796875" customWidth="1"/>
+    <col min="9" max="9" width="10.796875" customWidth="1"/>
+    <col min="10" max="10" width="22.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="str">
-        <v>TypeOfObject</v>
-      </c>
-      <c r="B1" s="1" t="str">
-        <v>NameOfObject</v>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="str">
-        <v>Remarks-FadaImport</v>
-      </c>
-      <c r="E1" s="1" t="str">
-        <v>FADA</v>
-      </c>
-      <c r="F1" s="1" t="str">
-        <v>Remarks-FADA</v>
-      </c>
-      <c r="G1" s="1" t="str">
-        <v>BioFresh</v>
-      </c>
-      <c r="H1" s="1" t="str">
-        <v>Remarks-BioFresh</v>
-      </c>
-      <c r="I1" s="1" t="str">
-        <v>DwC-A-export</v>
-      </c>
-      <c r="J1" s="1" t="str">
-        <v>Remarks-DwC-A-export</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="str">
-        <v>col.families</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="3" t="str">
-        <v>I would expect this table to be used during import when higher taxa are not found in the taxons table?</v>
-      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3"/>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="str">
-        <v>Surprised to see that this is directly used in the web-app</v>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="str">
-        <v>fada.archived_observations</v>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -219,12 +735,12 @@
       <c r="I3" s="2"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="str">
-        <v>fada.authors</v>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
@@ -241,12 +757,12 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="str">
-        <v>fada.bassins</v>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -259,12 +775,12 @@
       <c r="I5" s="2"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2" t="str">
-        <v>fada.biofresh_key_species</v>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
@@ -281,12 +797,12 @@
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="2" t="str">
-        <v>fada.biofresh_key_synonyms</v>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>2</v>
@@ -301,12 +817,12 @@
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="2" t="str">
-        <v>fada.biofresh_key_taxons</v>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>2</v>
@@ -321,12 +837,12 @@
       </c>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="2" t="str">
-        <v>fada.chapters</v>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -339,12 +855,12 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="2" t="str">
-        <v>fada.conservations</v>
+      <c r="B10" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -357,19 +873,17 @@
       <c r="I10" s="2"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="2" t="str">
-        <v>fada.distributions</v>
+      <c r="B11" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="3" t="str">
-        <v>Only consulted</v>
-      </c>
+      <c r="D11" s="3"/>
       <c r="E11" s="1" t="s">
         <v>2</v>
       </c>
@@ -379,12 +893,12 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2" t="str">
-        <v>fada.greferences</v>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>2</v>
@@ -399,12 +913,12 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="5" t="str">
-        <v>fada.genus_to_family</v>
+      <c r="B13" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -415,16 +929,16 @@
       <c r="I13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J13" s="1" t="str">
-        <v>Used in fada.fst_... Views</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="J13" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="2" t="str">
-        <v>fada.groups</v>
+      <c r="B14" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>2</v>
@@ -443,12 +957,12 @@
       </c>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="2" t="str">
-        <v>fada.groups_publications</v>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>2</v>
@@ -463,12 +977,12 @@
       <c r="I15" s="2"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="2" t="str">
-        <v>fada.groups_taxons</v>
+      <c r="B16" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -481,12 +995,12 @@
       <c r="I16" s="2"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="2" t="str">
-        <v>fada.groups_users</v>
+      <c r="B17" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -501,32 +1015,32 @@
       </c>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="2" t="str">
-        <v>fada.journals</v>
+      <c r="B18" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="1" t="str">
-        <v>Where used?</v>
+      <c r="F18" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="2"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="2" t="str">
-        <v>fada.locations</v>
+      <c r="B19" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -539,12 +1053,12 @@
       <c r="I19" s="2"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2" t="str">
-        <v>fada.observations</v>
+      <c r="B20" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>2</v>
@@ -561,12 +1075,12 @@
       <c r="I20" s="2"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="2" t="str">
-        <v>fada.observations_species</v>
+      <c r="B21" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>2</v>
@@ -583,12 +1097,12 @@
       <c r="I21" s="2"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="2" t="str">
-        <v>fada.obs_statuses</v>
+      <c r="B22" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -601,18 +1115,18 @@
       <c r="I22" s="2"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="2" t="str">
-        <v>fada.publications</v>
+      <c r="B23" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="4" t="str">
-        <v>Surprised to see this is in use, as I understood it was only created when the Rotifera data were processed &gt; possibility to reconcile together with greferences table??</v>
+      <c r="D23" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>2</v>
@@ -623,16 +1137,16 @@
       <c r="I23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J23" s="1" t="str">
-        <v>Not currently the case (Rotifera references stored in separate schema), but use is intended</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="J23" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="2" t="str">
-        <v>fada.ranks</v>
+      <c r="B24" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>2</v>
@@ -649,12 +1163,12 @@
       </c>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="2" t="str">
-        <v>fada.regions</v>
+      <c r="B25" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>2</v>
@@ -673,12 +1187,12 @@
       </c>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="2" t="str">
-        <v>fada.regions_species</v>
+      <c r="B26" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>2</v>
@@ -697,12 +1211,12 @@
       </c>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="2" t="str">
-        <v>fada.roles</v>
+      <c r="B27" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -715,12 +1229,12 @@
       <c r="I27" s="2"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="2" t="str">
-        <v>fada.roles_users</v>
+      <c r="B28" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -733,12 +1247,12 @@
       <c r="I28" s="2"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="2" t="str">
-        <v>fada.sites</v>
+      <c r="B29" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -751,12 +1265,12 @@
       <c r="I29" s="2"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="2" t="str">
-        <v>fada.species</v>
+      <c r="B30" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>2</v>
@@ -775,32 +1289,32 @@
       </c>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="2" t="str">
-        <v>fada.statuses</v>
+      <c r="B31" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="3" t="str">
-        <v>Wondering where this is used?</v>
+      <c r="F31" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="2"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="2" t="str">
-        <v>fada.synonyms</v>
+      <c r="B32" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>2</v>
@@ -817,12 +1331,12 @@
       </c>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="2" t="str">
-        <v>fada.taxons</v>
+      <c r="B33" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>2</v>
@@ -841,12 +1355,12 @@
       </c>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="2" t="str">
-        <v>fada.users</v>
+      <c r="B34" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -861,12 +1375,12 @@
       </c>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="2" t="str">
-        <v>fada.versions</v>
+      <c r="B35" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -879,12 +1393,12 @@
       <c r="I35" s="2"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="2" t="str">
-        <v>fada.biofresh_key_species_names</v>
+      <c r="B36" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -895,12 +1409,12 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="2" t="str">
-        <v>fada.fada_biofresh_export_id</v>
+      <c r="B37" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -911,12 +1425,12 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="2" t="str">
-        <v>fada.fada_export</v>
+      <c r="B38" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -931,12 +1445,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="2" t="str">
-        <v>fada.fada_export_region</v>
+      <c r="B39" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -951,30 +1465,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="2" t="str">
-        <v>fada.fadainfo</v>
+      <c r="B40" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="3" t="str">
-        <v>Surprised to see that none of these views is no longer in use, all directly called from BioFresh-portal app?</v>
+      <c r="H40" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="2" t="str">
-        <v>fada.families_with_no_htaxa</v>
+      <c r="B41" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -985,12 +1499,12 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="2" t="str">
-        <v>fada.fst_for_genus</v>
+      <c r="B42" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -1003,12 +1517,12 @@
       </c>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="2" t="str">
-        <v>fada.fst_for_tribe</v>
+      <c r="B43" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -1021,12 +1535,12 @@
       </c>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B44" s="2" t="str">
-        <v>fada.minitaxaview</v>
+      <c r="B44" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -1037,12 +1551,12 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="2" t="str">
-        <v>fada.originalnames</v>
+      <c r="B45" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -1053,12 +1567,12 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="2" t="str">
-        <v>fada.pubantoinsert</v>
+      <c r="B46" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1069,12 +1583,12 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B47" s="2" t="str">
-        <v>fada.pubsyntoinsert</v>
+      <c r="B47" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -1085,12 +1599,12 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="2" t="str">
-        <v>fada.refscnames</v>
+      <c r="B48" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -1101,12 +1615,12 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="2" t="str">
-        <v>fada.smallspecies</v>
+      <c r="B49" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -1117,12 +1631,12 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="2" t="str">
-        <v>fada.species_crosstab</v>
+      <c r="B50" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -1130,19 +1644,19 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
-      <c r="I50" s="4" t="str">
-        <v>??</v>
-      </c>
-      <c r="J50" s="4" t="str">
-        <v>Check, used for fst_for_genus OR genus_to_families table??</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
+      <c r="I50" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="2" t="str">
-        <v>fada.synonyms_split</v>
+      <c r="B51" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -1155,12 +1669,12 @@
       </c>
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="2" t="str">
-        <v>fada.view_groups</v>
+      <c r="B52" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -1171,12 +1685,12 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="2" t="str">
-        <v>fada.view_regions</v>
+      <c r="B53" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -1187,12 +1701,12 @@
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="2" t="str">
-        <v>fada.view_species</v>
+      <c r="B54" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -1203,12 +1717,12 @@
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="2" t="str">
-        <v>fada.view_taxons</v>
+      <c r="B55" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -1221,8 +1735,8 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="1" right="1" top="1.667" bottom="1.667" header="1" footer="1"/>
-  <pageSetup/>
+  <pageSetup orientation="portrait"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>